<commit_message>
fix export, optimalisasi sheet1 dan menambahkan sheet 2(kode area)
</commit_message>
<xml_diff>
--- a/recruitment_form.xlsx
+++ b/recruitment_form.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>No</t>
   </si>
@@ -96,42 +96,6 @@
   </si>
   <si>
     <t>Teknologi yang di Gunakan</t>
-  </si>
-  <si>
-    <t>Tawang</t>
-  </si>
-  <si>
-    <t>Cece Ruhyana, S.P</t>
-  </si>
-  <si>
-    <t>Harapan I</t>
-  </si>
-  <si>
-    <t>JL NOENGNOENG TISNA SAPUTRA RT 4 RW 16</t>
-  </si>
-  <si>
-    <t>Pemula</t>
-  </si>
-  <si>
-    <t>Jajar Legowo</t>
-  </si>
-  <si>
-    <t>Langkaplancar</t>
-  </si>
-  <si>
-    <t>Asep Sudrajat, M.T</t>
-  </si>
-  <si>
-    <t>Pakuan</t>
-  </si>
-  <si>
-    <t>jln pakuan indah</t>
-  </si>
-  <si>
-    <t>Profesional</t>
-  </si>
-  <si>
-    <t>codeigniter</t>
   </si>
 </sst>
 </file>
@@ -155,7 +119,7 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -170,16 +134,14 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF009343"/>
+        <bgColor rgb="FF009343"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <bottom style="thick">
-        <color rgb="FF#00FF00"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -188,7 +150,7 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -490,16 +452,13 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="3.427734" bestFit="true" customWidth="true" style="0"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
@@ -585,82 +544,6 @@
       </c>
       <c r="AB1" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
-        <v>3278040</v>
-      </c>
-      <c r="D2">
-        <v>3278040001</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J2">
-        <v>1982</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M2">
-        <v>340</v>
-      </c>
-      <c r="N2">
-        <v>2007</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3">
-        <v>3206090</v>
-      </c>
-      <c r="D3">
-        <v>3206090007</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3">
-        <v>2011</v>
-      </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3">
-        <v>2000</v>
-      </c>
-      <c r="N3">
-        <v>2021</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>